<commit_message>
Help and Support feature updated
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp_Android_Identifiers.xlsx
+++ b/Selenium-Scripts/src/DigitalApp_Android_Identifiers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
   <si>
     <t>Key</t>
   </si>
@@ -334,6 +334,39 @@
   </si>
   <si>
     <t>//android.widget.Button[@text='PLACE ORDER']</t>
+  </si>
+  <si>
+    <t>//android.widget.FrameLayout[1]/android.view.ViewGroup/android.widget.TextView</t>
+  </si>
+  <si>
+    <t>quickLink</t>
+  </si>
+  <si>
+    <t>quickLinkQuestion</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='I am migrating my line. Does it affect my ICP subscription?']</t>
+  </si>
+  <si>
+    <t>//android.view.ViewGroup[2]/android.widget.TextView</t>
+  </si>
+  <si>
+    <t>quickLinkQuestion2</t>
+  </si>
+  <si>
+    <t>//androidx.recyclerview.widget.RecyclerView[2]/android.view.ViewGroup[1]</t>
+  </si>
+  <si>
+    <t>FromEtisalatShop</t>
+  </si>
+  <si>
+    <t>ShopPage</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='All Devices']</t>
+  </si>
+  <si>
+    <t>TopMenu</t>
   </si>
 </sst>
 </file>
@@ -436,7 +469,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -447,6 +480,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -871,16 +907,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="2" max="2" width="93.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -963,8 +999,57 @@
         <v>38</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -972,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,7 +1197,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Migration feature file update
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp_Android_Identifiers.xlsx
+++ b/Selenium-Scripts/src/DigitalApp_Android_Identifiers.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
     <sheet name="RechargeHistoryPage" sheetId="15" r:id="rId2"/>
     <sheet name="HelpAndSupportPage" sheetId="10" r:id="rId3"/>
-    <sheet name="MigrationPage" sheetId="13" r:id="rId4"/>
-    <sheet name="PlansAndAddonsPage" sheetId="14" r:id="rId5"/>
-    <sheet name="FeedBackPage" sheetId="7" r:id="rId6"/>
-    <sheet name="StartingPage" sheetId="3" r:id="rId7"/>
-    <sheet name="LoginPage" sheetId="4" r:id="rId8"/>
-    <sheet name="HomeMovePage" sheetId="11" r:id="rId9"/>
-    <sheet name="HomeMoveOrderTrackingPage" sheetId="16" r:id="rId10"/>
-    <sheet name="Menu" sheetId="5" r:id="rId11"/>
-    <sheet name="detailsPage" sheetId="12" r:id="rId12"/>
+    <sheet name="UDMigrationPPMPage" sheetId="13" r:id="rId4"/>
+    <sheet name="UDMigrationCR2Page" sheetId="17" r:id="rId5"/>
+    <sheet name="PlansAndAddonsPage" sheetId="14" r:id="rId6"/>
+    <sheet name="FeedBackPage" sheetId="7" r:id="rId7"/>
+    <sheet name="StartingPage" sheetId="3" r:id="rId8"/>
+    <sheet name="LoginPage" sheetId="4" r:id="rId9"/>
+    <sheet name="HomeMovePage" sheetId="11" r:id="rId10"/>
+    <sheet name="HomeMoveOrderTrackingPage" sheetId="16" r:id="rId11"/>
+    <sheet name="Menu" sheetId="5" r:id="rId12"/>
+    <sheet name="detailsPage" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="166">
   <si>
     <t>Key</t>
   </si>
@@ -516,6 +517,18 @@
   </si>
   <si>
     <t>StatusAndSubStatus</t>
+  </si>
+  <si>
+    <t>AECBCheck</t>
+  </si>
+  <si>
+    <t>BillSummaryPage</t>
+  </si>
+  <si>
+    <t>ConfirmButton</t>
+  </si>
+  <si>
+    <t>RequestForChangePlan</t>
   </si>
 </sst>
 </file>
@@ -1004,9 +1017,239 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1102,7 +1345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1145,7 +1388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1423,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1555,6 +1798,11 @@
         <v>96</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1562,10 +1810,166 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1695,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1752,7 +2156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1818,234 +2222,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
elife change plan update
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/DigitalApp_Android_Identifiers.xlsx
+++ b/Selenium-Scripts/src/DigitalApp_Android_Identifiers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,15 @@
     <sheet name="HelpAndSupportPage" sheetId="10" r:id="rId3"/>
     <sheet name="UDMigrationPPMPage" sheetId="13" r:id="rId4"/>
     <sheet name="UDMigrationCR2Page" sheetId="17" r:id="rId5"/>
-    <sheet name="PlansAndAddonsPage" sheetId="14" r:id="rId6"/>
-    <sheet name="FeedBackPage" sheetId="7" r:id="rId7"/>
-    <sheet name="StartingPage" sheetId="3" r:id="rId8"/>
-    <sheet name="LoginPage" sheetId="4" r:id="rId9"/>
-    <sheet name="HomeMovePage" sheetId="11" r:id="rId10"/>
-    <sheet name="HomeMoveOrderTrackingPage" sheetId="16" r:id="rId11"/>
-    <sheet name="Menu" sheetId="5" r:id="rId12"/>
-    <sheet name="detailsPage" sheetId="12" r:id="rId13"/>
+    <sheet name="elifeChangePlanPage" sheetId="18" r:id="rId6"/>
+    <sheet name="PlansAndAddonsPage" sheetId="14" r:id="rId7"/>
+    <sheet name="FeedBackPage" sheetId="7" r:id="rId8"/>
+    <sheet name="StartingPage" sheetId="3" r:id="rId9"/>
+    <sheet name="LoginPage" sheetId="4" r:id="rId10"/>
+    <sheet name="HomeMovePage" sheetId="11" r:id="rId11"/>
+    <sheet name="HomeMoveOrderTrackingPage" sheetId="16" r:id="rId12"/>
+    <sheet name="Menu" sheetId="5" r:id="rId13"/>
+    <sheet name="detailsPage" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="202">
   <si>
     <t>Key</t>
   </si>
@@ -529,13 +530,308 @@
   </si>
   <si>
     <t>RequestForChangePlan</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text='Etisalat Shop']</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>//android.widget.LinearLayout[@index=0]//android.widget.TextView[@text='Home']</t>
+  </si>
+  <si>
+    <r>
+      <t>changePlan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>elife4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>unlimitedpkg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TargetPackage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>speed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rental</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>commitment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>noCommitment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>continue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>miniPack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>telephone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>stb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>router</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>optionAddons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>currentPlan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>newPlan</t>
+  </si>
+  <si>
+    <r>
+      <t>general</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>termsAndConditions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>termsAndConditions</t>
+  </si>
+  <si>
+    <t>alreadyexist</t>
+  </si>
+  <si>
+    <t>newlyCaptured</t>
+  </si>
+  <si>
+    <t>freedelievry</t>
+  </si>
+  <si>
+    <t>installationDate</t>
+  </si>
+  <si>
+    <t>reviewDetail</t>
+  </si>
+  <si>
+    <t>confirmRequest</t>
+  </si>
+  <si>
+    <t>SuccessMsg</t>
+  </si>
+  <si>
+    <t>woCreation</t>
+  </si>
+  <si>
+    <t>newPackage</t>
+  </si>
+  <si>
+    <t>montlyCharges</t>
+  </si>
+  <si>
+    <t>proratedCharges</t>
+  </si>
+  <si>
+    <t>monthlyRentalCharges</t>
+  </si>
+  <si>
+    <t>ExistCharges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,8 +885,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF080808"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,8 +905,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -612,8 +920,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -630,8 +953,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -646,8 +970,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="16" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="17">
     <cellStyle name="Hyperlink 2" xfId="5"/>
     <cellStyle name="Hyperlink 2 2" xfId="11"/>
     <cellStyle name="Hyperlink 3" xfId="3"/>
@@ -664,6 +996,7 @@
     <cellStyle name="Normal 6" xfId="14"/>
     <cellStyle name="Normal 7" xfId="1"/>
     <cellStyle name="Normal 8" xfId="15"/>
+    <cellStyle name="Normal 9" xfId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,13 +1280,13 @@
       <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -961,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -969,7 +1302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -977,7 +1310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -985,7 +1318,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -993,7 +1326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1001,7 +1334,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1017,19 +1350,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1037,207 +1370,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1247,19 +1418,19 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="78" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1267,77 +1438,207 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1347,19 +1648,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1367,20 +1668,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1390,19 +1748,62 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="81" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1410,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1418,7 +1819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1426,7 +1827,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1447,13 +1848,13 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.109375" customWidth="1"/>
     <col min="2" max="2" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1469,7 +1870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1477,7 +1878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1485,12 +1886,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -1508,13 +1909,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
     <col min="2" max="2" width="93.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1530,7 +1931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1538,7 +1939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1546,7 +1947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1554,7 +1955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1562,7 +1963,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1570,7 +1971,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1578,7 +1979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1586,7 +1987,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1594,7 +1995,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -1602,7 +2003,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1610,7 +2011,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -1618,7 +2019,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -1626,7 +2027,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -1634,7 +2035,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -1642,7 +2043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
@@ -1650,7 +2051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -1672,13 +2073,13 @@
       <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27.5546875" customWidth="1"/>
     <col min="2" max="2" width="72" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1694,7 +2095,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1702,7 +2103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1710,7 +2111,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1718,7 +2119,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1726,7 +2127,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1734,7 +2135,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1742,7 +2143,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -1750,7 +2151,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1758,7 +2159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1766,7 +2167,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1774,7 +2175,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1782,7 +2183,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1790,7 +2191,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1798,7 +2199,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -1812,17 +2213,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27.5546875" customWidth="1"/>
     <col min="2" max="2" width="72" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1830,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1838,7 +2239,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1846,7 +2247,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1854,7 +2255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1862,7 +2263,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1870,7 +2271,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1878,7 +2279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1886,7 +2287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -1894,7 +2295,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1902,7 +2303,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1910,7 +2311,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1918,7 +2319,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1926,7 +2327,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1934,7 +2335,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1942,19 +2343,19 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>165</v>
       </c>
@@ -1966,19 +2367,254 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="11"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27.5546875" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1986,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1994,7 +2630,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -2002,7 +2638,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -2010,7 +2646,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.6" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>115</v>
       </c>
@@ -2018,7 +2654,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2026,7 +2662,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2034,7 +2670,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -2042,7 +2678,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -2056,7 +2692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2064,13 +2700,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
     <col min="2" max="2" width="81.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2086,7 +2722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2099,7 +2735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2107,13 +2743,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2129,7 +2765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -2140,7 +2776,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2149,74 +2785,6 @@
       </c>
       <c r="C4" t="s">
         <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>